<commit_message>
Added Offcanvas Navigation bar. Checking  web and mobile version. WIP
</commit_message>
<xml_diff>
--- a/src/USD_Inflation.xlsx
+++ b/src/USD_Inflation.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sveta/Svetas_project/time_convert_app/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893F2CB1-1A74-0F4A-BA51-BF8892A7BFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="01"/>
+    <sheet name="01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,8 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -70,7 +88,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -104,16 +122,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -122,34 +140,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -160,10 +181,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -201,71 +222,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -293,7 +314,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -316,11 +337,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -329,13 +350,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -345,7 +366,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -354,7 +375,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -363,7 +384,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -371,10 +392,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -439,21 +460,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1960</v>
       </c>
@@ -469,508 +492,508 @@
         <v>1.45797598627791</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <f>A2+1</f>
+        <v>1961</v>
       </c>
       <c r="B3" s="3">
         <v>1.07072414764724</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <f>A3+1</f>
+        <v>1962</v>
       </c>
       <c r="B4" s="3">
-        <v>1.19877334820186</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+        <v>1.1987733482018601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f>A4+1</f>
+        <v>1963</v>
       </c>
       <c r="B5" s="3">
-        <v>1.23966942148753</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+        <v>1.2396694214875299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <f>A5+1</f>
+        <v>1964</v>
       </c>
       <c r="B6" s="3">
-        <v>1.27891156462591</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+        <v>1.2789115646259099</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <f>A6+1</f>
+        <v>1965</v>
       </c>
       <c r="B7" s="3">
-        <v>1.58516926383662</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+        <v>1.5851692638366199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <f>A7+1</f>
+        <v>1966</v>
       </c>
       <c r="B8" s="3">
-        <v>3.0150753768844</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+        <v>3.0150753768844001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <f>A8+1</f>
+        <v>1967</v>
       </c>
       <c r="B9" s="3">
-        <v>2.77278562259309</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+        <v>2.7727856225930898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <f>A9+1</f>
+        <v>1968</v>
       </c>
       <c r="B10" s="3">
-        <v>4.27179615288537</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+        <v>4.2717961528853703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f>A10+1</f>
+        <v>1969</v>
       </c>
       <c r="B11" s="3">
-        <v>5.46238620028745</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+        <v>5.4623862002874501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <f>A11+1</f>
+        <v>1970</v>
       </c>
       <c r="B12" s="3">
-        <v>5.83825533848251</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+        <v>5.8382553384825098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <f>A12+1</f>
+        <v>1971</v>
       </c>
       <c r="B13" s="3">
-        <v>4.29276668813051</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+        <v>4.2927666881305102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <f>A13+1</f>
+        <v>1972</v>
       </c>
       <c r="B14" s="3">
-        <v>3.27227824655283</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+        <v>3.2722782465528302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <f>A14+1</f>
+        <v>1973</v>
       </c>
       <c r="B15" s="3">
-        <v>6.17776006377038</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+        <v>6.1777600637703802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f>A15+1</f>
+        <v>1974</v>
       </c>
       <c r="B16" s="3">
         <v>11.0548048048048</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f>A16+1</f>
+        <v>1975</v>
       </c>
       <c r="B17" s="3">
-        <v>9.14314686496535</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+        <v>9.1431468649653507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <f>A17+1</f>
+        <v>1976</v>
       </c>
       <c r="B18" s="3">
-        <v>5.74481263549085</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+        <v>5.7448126354908498</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <f>A18+1</f>
+        <v>1977</v>
       </c>
       <c r="B19" s="3">
         <v>6.5016839947284</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <f>A19+1</f>
+        <v>1978</v>
       </c>
       <c r="B20" s="3">
-        <v>7.63096383885606</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+        <v>7.6309638388560597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <f>A20+1</f>
+        <v>1979</v>
       </c>
       <c r="B21" s="3">
         <v>11.2544711292795</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <f>A21+1</f>
+        <v>1980</v>
       </c>
       <c r="B22" s="3">
-        <v>13.5492019749684</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+        <v>13.549201974968399</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <f>A22+1</f>
+        <v>1981</v>
       </c>
       <c r="B23" s="3">
         <v>10.3347153402771</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <f>A23+1</f>
+        <v>1982</v>
       </c>
       <c r="B24" s="3">
-        <v>6.13142700027493</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+        <v>6.1314270002749298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <f>A24+1</f>
+        <v>1983</v>
       </c>
       <c r="B25" s="3">
         <v>3.21243523316065</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <f>A25+1</f>
+        <v>1984</v>
       </c>
       <c r="B26" s="3">
-        <v>4.30053547523429</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+        <v>4.3005354752342901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <f>A26+1</f>
+        <v>1985</v>
       </c>
       <c r="B27" s="3">
-        <v>3.54564415209365</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+        <v>3.5456441520936499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <f>A27+1</f>
+        <v>1986</v>
       </c>
       <c r="B28" s="3">
-        <v>1.89804772234276</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+        <v>1.8980477223427601</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <f>A28+1</f>
+        <v>1987</v>
       </c>
       <c r="B29" s="3">
-        <v>3.6645632175169</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+        <v>3.6645632175168998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <f>A29+1</f>
+        <v>1988</v>
       </c>
       <c r="B30" s="3">
-        <v>4.07774110744413</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+        <v>4.0777411074441297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <f>A30+1</f>
+        <v>1989</v>
       </c>
       <c r="B31" s="3">
-        <v>4.82700303008944</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+        <v>4.8270030300894398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <f>A31+1</f>
+        <v>1990</v>
       </c>
       <c r="B32" s="3">
-        <v>5.39795643990325</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+        <v>5.3979564399032496</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <f>A32+1</f>
+        <v>1991</v>
       </c>
       <c r="B33" s="3">
-        <v>4.23496396453849</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+        <v>4.2349639645384904</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <f>A33+1</f>
+        <v>1992</v>
       </c>
       <c r="B34" s="3">
-        <v>3.02881967814969</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+        <v>3.0288196781496901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <f>A34+1</f>
+        <v>1993</v>
       </c>
       <c r="B35" s="3">
-        <v>2.95165696638559</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+        <v>2.9516569663855901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <f>A35+1</f>
+        <v>1994</v>
       </c>
       <c r="B36" s="3">
         <v>2.60744159215453</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row r="37" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <f>A36+1</f>
+        <v>1995</v>
       </c>
       <c r="B37" s="3">
-        <v>2.80541968853662</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+        <v>2.8054196885366198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <f>A37+1</f>
+        <v>1996</v>
       </c>
       <c r="B38" s="3">
-        <v>2.93120419993441</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+        <v>2.9312041999344101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <f>A38+1</f>
+        <v>1997</v>
       </c>
       <c r="B39" s="3">
-        <v>2.33768993730735</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+        <v>2.3376899373073501</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <f>A39+1</f>
+        <v>1998</v>
       </c>
       <c r="B40" s="3">
-        <v>1.55227909874364</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+        <v>1.5522790987436399</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <f>A40+1</f>
+        <v>1999</v>
       </c>
       <c r="B41" s="3">
-        <v>2.18802719697358</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+        <v>2.1880271969735801</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <f>A41+1</f>
+        <v>2000</v>
       </c>
       <c r="B42" s="3">
-        <v>3.37685727149929</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+        <v>3.3768572714992899</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <f>A42+1</f>
+        <v>2001</v>
       </c>
       <c r="B43" s="3">
-        <v>2.82617111885407</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+        <v>2.8261711188540701</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <f>A43+1</f>
+        <v>2002</v>
       </c>
       <c r="B44" s="3">
-        <v>1.58603162650601</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+        <v>1.5860316265060099</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <f>A44+1</f>
+        <v>2003</v>
       </c>
       <c r="B45" s="3">
-        <v>2.27009497336115</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+        <v>2.2700949733611502</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <f>A45+1</f>
+        <v>2004</v>
       </c>
       <c r="B46" s="3">
-        <v>2.67723669309172</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+        <v>2.6772366930917202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <f>A46+1</f>
+        <v>2005</v>
       </c>
       <c r="B47" s="3">
-        <v>3.3927468454955</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+        <v>3.3927468454955001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <f>A47+1</f>
+        <v>2006</v>
       </c>
       <c r="B48" s="3">
-        <v>3.22594410070404</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+        <v>3.2259441007040399</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <f>A48+1</f>
+        <v>2007</v>
       </c>
       <c r="B49" s="3">
-        <v>2.85267248150138</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+        <v>2.8526724815013802</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <f>A49+1</f>
+        <v>2008</v>
       </c>
       <c r="B50" s="3">
-        <v>3.839100296651</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+        <v>3.8391002966509999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <f>A50+1</f>
+        <v>2009</v>
       </c>
       <c r="B51" s="3">
         <v>-0.355546266299747</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
+    <row r="52" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <f>A51+1</f>
+        <v>2010</v>
       </c>
       <c r="B52" s="3">
         <v>1.6400434423899</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
+    <row r="53" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <f>A52+1</f>
+        <v>2011</v>
       </c>
       <c r="B53" s="3">
-        <v>3.156841568622</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
+        <v>3.1568415686220002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <f>A53+1</f>
+        <v>2012</v>
       </c>
       <c r="B54" s="3">
-        <v>2.06933726526067</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
+        <v>2.0693372652606699</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <f>A54+1</f>
+        <v>2013</v>
       </c>
       <c r="B55" s="3">
         <v>1.46483265562717</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
+    <row r="56" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <f>A55+1</f>
+        <v>2014</v>
       </c>
       <c r="B56" s="3">
         <v>1.62222297740817</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
+    <row r="57" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <f>A56+1</f>
+        <v>2015</v>
       </c>
       <c r="B57" s="3">
         <v>0.118627135552451</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
+    <row r="58" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <f>A57+1</f>
+        <v>2016</v>
       </c>
       <c r="B58" s="3">
         <v>1.26158320570536</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
+    <row r="59" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <f>A58+1</f>
+        <v>2017</v>
       </c>
       <c r="B59" s="3">
-        <v>2.13011000365961</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
+        <v>2.1301100036596101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <f>A59+1</f>
+        <v>2018</v>
       </c>
       <c r="B60" s="3">
         <v>2.44258329692817</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
+    <row r="61" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <f>A60+1</f>
+        <v>2019</v>
       </c>
       <c r="B61" s="3">
-        <v>1.81221007526021</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
+        <v>1.8122100752602099</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <f>A61+1</f>
+        <v>2020</v>
       </c>
       <c r="B62" s="3">
         <v>1.23358439630629</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
+    <row r="63" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <f>A62+1</f>
+        <v>2021</v>
       </c>
       <c r="B63" s="3">
-        <v>4.69785886363742</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
+        <v>4.6978588636374203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <f>A63+1</f>
+        <v>2022</v>
       </c>
       <c r="B64" s="3">
-        <v>8.00279982052121</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
+        <v>8.0027998205212096</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2023</v>
       </c>
       <c r="B65" s="4">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new EUR and RUB data
</commit_message>
<xml_diff>
--- a/src/USD_Inflation.xlsx
+++ b/src/USD_Inflation.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>USD_Inflation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>year</t>
   </si>
@@ -29,11 +26,11 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -41,13 +38,17 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -66,8 +67,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -125,21 +132,6 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -165,60 +157,36 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -237,19 +205,20 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Blank">
+    <a:clrScheme name="Office Theme">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -257,10 +226,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -287,7 +256,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Blank">
+    <a:fontScheme name="Office Theme">
       <a:majorFont>
         <a:latin typeface="Helvetica Neue"/>
         <a:ea typeface="Helvetica Neue"/>
@@ -299,7 +268,7 @@
         <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Blank">
+    <a:fmtScheme name="Office Theme">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -372,13 +341,31 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -437,47 +424,56 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -725,14 +721,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1017,11 +1019,11 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1045,10 +1047,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1299,772 +1301,555 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:E68"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.67188" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.85156" style="1" customWidth="1"/>
-    <col min="3" max="5" width="8.35156" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+      <c r="A2" s="3">
+        <v>1960</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
       <c r="A3" s="5">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="B3" s="6">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="5">
+        <v>1962</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="5">
+        <v>1963</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="5">
+        <v>1964</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="5">
+        <v>1965</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="5">
+        <v>1966</v>
+      </c>
+      <c r="B8" s="6">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="5">
+        <v>1967</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="5">
+        <v>1968</v>
+      </c>
+      <c r="B10" s="6">
+        <v>4.27</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="5">
+        <v>1969</v>
+      </c>
+      <c r="B11" s="6">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="5">
+        <v>1970</v>
+      </c>
+      <c r="B12" s="6">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="5">
+        <v>1971</v>
+      </c>
+      <c r="B13" s="6">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="5">
+        <v>1972</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="5">
+        <v>1973</v>
+      </c>
+      <c r="B15" s="6">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="5">
+        <v>1974</v>
+      </c>
+      <c r="B16" s="6">
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="5">
+        <v>1975</v>
+      </c>
+      <c r="B17" s="6">
+        <v>9.140000000000001</v>
+      </c>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="5">
+        <v>1976</v>
+      </c>
+      <c r="B18" s="6">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" s="5">
+        <v>1977</v>
+      </c>
+      <c r="B19" s="6">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" s="5">
+        <v>1978</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7.63</v>
+      </c>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" s="5">
+        <v>1979</v>
+      </c>
+      <c r="B21" s="6">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" s="5">
+        <v>1980</v>
+      </c>
+      <c r="B22" s="6">
+        <v>13.55</v>
+      </c>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" s="5">
+        <v>1981</v>
+      </c>
+      <c r="B23" s="6">
+        <v>10.33</v>
+      </c>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" s="5">
+        <v>1982</v>
+      </c>
+      <c r="B24" s="6">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" s="5">
+        <v>1983</v>
+      </c>
+      <c r="B25" s="6">
+        <v>3.21</v>
+      </c>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" s="5">
+        <v>1984</v>
+      </c>
+      <c r="B26" s="6">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" s="5">
+        <v>1985</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" s="5">
+        <v>1986</v>
+      </c>
+      <c r="B28" s="6">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" s="5">
+        <v>1987</v>
+      </c>
+      <c r="B29" s="6">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" s="5">
+        <v>1988</v>
+      </c>
+      <c r="B30" s="6">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" s="5">
+        <v>1989</v>
+      </c>
+      <c r="B31" s="6">
+        <v>4.83</v>
+      </c>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" s="5">
+        <v>1990</v>
+      </c>
+      <c r="B32" s="6">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" s="5">
+        <v>1991</v>
+      </c>
+      <c r="B33" s="6">
+        <v>4.23</v>
+      </c>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" s="5">
+        <v>1992</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" s="5">
+        <v>1993</v>
+      </c>
+      <c r="B35" s="6">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" s="5">
+        <v>1994</v>
+      </c>
+      <c r="B36" s="6">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" s="5">
+        <v>1995</v>
+      </c>
+      <c r="B37" s="6">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" s="5">
+        <v>1996</v>
+      </c>
+      <c r="B38" s="6">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" s="5">
+        <v>1997</v>
+      </c>
+      <c r="B39" s="6">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" s="5">
+        <v>1998</v>
+      </c>
+      <c r="B40" s="6">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" s="5">
+        <v>1999</v>
+      </c>
+      <c r="B41" s="6">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B42" s="6">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="43" ht="20.05" customHeight="1">
+      <c r="A43" s="5">
+        <v>2001</v>
+      </c>
+      <c r="B43" s="6">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
+      <c r="A44" s="5">
+        <v>2002</v>
+      </c>
+      <c r="B44" s="6">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="45" ht="20.05" customHeight="1">
+      <c r="A45" s="5">
+        <v>2003</v>
+      </c>
+      <c r="B45" s="6">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="46" ht="20.05" customHeight="1">
+      <c r="A46" s="5">
+        <v>2004</v>
+      </c>
+      <c r="B46" s="6">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="47" ht="20.05" customHeight="1">
+      <c r="A47" s="5">
+        <v>2005</v>
+      </c>
+      <c r="B47" s="6">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="48" ht="20.05" customHeight="1">
+      <c r="A48" s="5">
+        <v>2006</v>
+      </c>
+      <c r="B48" s="6">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="49" ht="20.05" customHeight="1">
+      <c r="A49" s="5">
+        <v>2007</v>
+      </c>
+      <c r="B49" s="6">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="50" ht="20.05" customHeight="1">
+      <c r="A50" s="5">
+        <v>2008</v>
+      </c>
+      <c r="B50" s="6">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="51" ht="20.05" customHeight="1">
+      <c r="A51" s="5">
+        <v>2009</v>
+      </c>
+      <c r="B51" s="6">
+        <v>-0.36</v>
+      </c>
+    </row>
+    <row r="52" ht="20.05" customHeight="1">
+      <c r="A52" s="5">
+        <v>2010</v>
+      </c>
+      <c r="B52" s="6">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="53" ht="20.05" customHeight="1">
+      <c r="A53" s="5">
+        <v>2011</v>
+      </c>
+      <c r="B53" s="6">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="54" ht="20.05" customHeight="1">
+      <c r="A54" s="5">
+        <v>2012</v>
+      </c>
+      <c r="B54" s="6">
+        <v>2.07</v>
+      </c>
+    </row>
+    <row r="55" ht="20.05" customHeight="1">
+      <c r="A55" s="5">
+        <v>2013</v>
+      </c>
+      <c r="B55" s="6">
         <v>1.46</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8">
-        <v>1961</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1.07</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="8">
-        <v>1962</v>
-      </c>
-      <c r="B5" s="9">
-        <v>1.2</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8">
-        <v>1963</v>
-      </c>
-      <c r="B6" s="9">
-        <v>1.24</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="8">
-        <v>1964</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1.28</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8">
-        <v>1965</v>
-      </c>
-      <c r="B8" s="9">
-        <v>1.59</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8">
-        <v>1966</v>
-      </c>
-      <c r="B9" s="9">
-        <v>3.02</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="8">
-        <v>1967</v>
-      </c>
-      <c r="B10" s="9">
-        <v>2.77</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="8">
-        <v>1968</v>
-      </c>
-      <c r="B11" s="9">
-        <v>4.27</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="8">
-        <v>1969</v>
-      </c>
-      <c r="B12" s="9">
-        <v>5.46</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="8">
-        <v>1970</v>
-      </c>
-      <c r="B13" s="9">
-        <v>5.84</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="8">
-        <v>1971</v>
-      </c>
-      <c r="B14" s="9">
-        <v>4.29</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="8">
-        <v>1972</v>
-      </c>
-      <c r="B15" s="9">
-        <v>3.27</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="8">
-        <v>1973</v>
-      </c>
-      <c r="B16" s="9">
-        <v>6.18</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="8">
-        <v>1974</v>
-      </c>
-      <c r="B17" s="9">
-        <v>11.05</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="8">
-        <v>1975</v>
-      </c>
-      <c r="B18" s="9">
-        <v>9.140000000000001</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="8">
-        <v>1976</v>
-      </c>
-      <c r="B19" s="9">
-        <v>5.74</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="8">
-        <v>1977</v>
-      </c>
-      <c r="B20" s="9">
-        <v>6.5</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="8">
-        <v>1978</v>
-      </c>
-      <c r="B21" s="9">
-        <v>7.63</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="8">
-        <v>1979</v>
-      </c>
-      <c r="B22" s="9">
-        <v>11.25</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="8">
-        <v>1980</v>
-      </c>
-      <c r="B23" s="9">
-        <v>13.55</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="8">
-        <v>1981</v>
-      </c>
-      <c r="B24" s="9">
-        <v>10.33</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="8">
-        <v>1982</v>
-      </c>
-      <c r="B25" s="9">
-        <v>6.13</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="8">
-        <v>1983</v>
-      </c>
-      <c r="B26" s="9">
-        <v>3.21</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="8">
-        <v>1984</v>
-      </c>
-      <c r="B27" s="9">
-        <v>4.3</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="8">
-        <v>1985</v>
-      </c>
-      <c r="B28" s="9">
-        <v>3.55</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="8">
-        <v>1986</v>
-      </c>
-      <c r="B29" s="9">
-        <v>1.9</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="8">
-        <v>1987</v>
-      </c>
-      <c r="B30" s="9">
-        <v>3.66</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="8">
-        <v>1988</v>
-      </c>
-      <c r="B31" s="9">
-        <v>4.08</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" s="8">
-        <v>1989</v>
-      </c>
-      <c r="B32" s="9">
-        <v>4.83</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" s="8">
-        <v>1990</v>
-      </c>
-      <c r="B33" s="9">
-        <v>5.4</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" s="8">
-        <v>1991</v>
-      </c>
-      <c r="B34" s="9">
-        <v>4.23</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" s="8">
-        <v>1992</v>
-      </c>
-      <c r="B35" s="9">
-        <v>3.03</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" s="8">
-        <v>1993</v>
-      </c>
-      <c r="B36" s="9">
-        <v>2.95</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" s="8">
-        <v>1994</v>
-      </c>
-      <c r="B37" s="9">
-        <v>2.61</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" s="8">
-        <v>1995</v>
-      </c>
-      <c r="B38" s="9">
-        <v>2.81</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" s="8">
-        <v>1996</v>
-      </c>
-      <c r="B39" s="9">
-        <v>2.93</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" s="8">
-        <v>1997</v>
-      </c>
-      <c r="B40" s="9">
-        <v>2.34</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" s="8">
-        <v>1998</v>
-      </c>
-      <c r="B41" s="9">
-        <v>1.55</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" s="8">
-        <v>1999</v>
-      </c>
-      <c r="B42" s="9">
-        <v>2.19</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" s="8">
-        <v>2000</v>
-      </c>
-      <c r="B43" s="9">
-        <v>3.38</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" s="8">
-        <v>2001</v>
-      </c>
-      <c r="B44" s="9">
-        <v>2.83</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" s="8">
-        <v>2002</v>
-      </c>
-      <c r="B45" s="9">
-        <v>1.59</v>
-      </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" s="8">
-        <v>2003</v>
-      </c>
-      <c r="B46" s="9">
-        <v>2.27</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" s="8">
-        <v>2004</v>
-      </c>
-      <c r="B47" s="9">
-        <v>2.68</v>
-      </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" s="8">
-        <v>2005</v>
-      </c>
-      <c r="B48" s="9">
-        <v>3.39</v>
-      </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" s="8">
-        <v>2006</v>
-      </c>
-      <c r="B49" s="9">
-        <v>3.23</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" s="8">
-        <v>2007</v>
-      </c>
-      <c r="B50" s="9">
-        <v>2.85</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-    </row>
-    <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" s="8">
-        <v>2008</v>
-      </c>
-      <c r="B51" s="9">
-        <v>3.84</v>
-      </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" s="8">
-        <v>2009</v>
-      </c>
-      <c r="B52" s="9">
-        <v>-0.36</v>
-      </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" s="8">
-        <v>2010</v>
-      </c>
-      <c r="B53" s="9">
-        <v>1.64</v>
-      </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" s="8">
-        <v>2011</v>
-      </c>
-      <c r="B54" s="9">
-        <v>3.16</v>
-      </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" s="8">
-        <v>2012</v>
-      </c>
-      <c r="B55" s="9">
-        <v>2.07</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" s="8">
-        <v>2013</v>
-      </c>
-      <c r="B56" s="9">
-        <v>1.46</v>
-      </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-    </row>
-    <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" s="8">
+    </row>
+    <row r="56" ht="30" customHeight="1">
+      <c r="A56" s="5">
         <v>2014</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B56" s="6">
         <v>1.62</v>
       </c>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" s="8">
+    </row>
+    <row r="57" ht="30" customHeight="1">
+      <c r="A57" s="5">
         <v>2015</v>
       </c>
-      <c r="B58" s="9">
+      <c r="B57" s="6">
         <v>0.12</v>
       </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" s="8">
+    </row>
+    <row r="58" ht="30" customHeight="1">
+      <c r="A58" s="5">
         <v>2016</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B58" s="6">
         <v>1.26</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-    </row>
-    <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" s="8">
+    </row>
+    <row r="59" ht="30" customHeight="1">
+      <c r="A59" s="5">
         <v>2017</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B59" s="6">
         <v>2.13</v>
       </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-    </row>
-    <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" s="8">
+    </row>
+    <row r="60" ht="30" customHeight="1">
+      <c r="A60" s="5">
         <v>2018</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B60" s="6">
         <v>2.44</v>
       </c>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-    </row>
-    <row r="62" ht="20.05" customHeight="1">
-      <c r="A62" s="8">
+    </row>
+    <row r="61" ht="30" customHeight="1">
+      <c r="A61" s="5">
         <v>2019</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B61" s="6">
         <v>1.81</v>
       </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-    </row>
-    <row r="63" ht="20.05" customHeight="1">
-      <c r="A63" s="8">
+    </row>
+    <row r="62" ht="30" customHeight="1">
+      <c r="A62" s="5">
         <v>2020</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B62" s="6">
         <v>1.23</v>
       </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-    </row>
-    <row r="64" ht="20.05" customHeight="1">
-      <c r="A64" s="8">
+    </row>
+    <row r="63" ht="30" customHeight="1">
+      <c r="A63" s="5">
         <v>2021</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B63" s="6">
         <v>4.7</v>
       </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" ht="20.05" customHeight="1">
-      <c r="A65" s="8">
+    </row>
+    <row r="64" ht="30" customHeight="1">
+      <c r="A64" s="5">
         <v>2022</v>
       </c>
-      <c r="B65" s="9">
+      <c r="B64" s="7">
         <v>8</v>
       </c>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" ht="20.05" customHeight="1">
-      <c r="A66" s="8">
+    </row>
+    <row r="65" ht="30" customHeight="1">
+      <c r="A65" s="5">
         <v>2023</v>
       </c>
-      <c r="B66" s="9">
-        <v>5.8</v>
-      </c>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
+      <c r="B65" s="6">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="66" ht="30" customHeight="1">
+      <c r="A66" s="5">
+        <v>2024</v>
+      </c>
+      <c r="B66" s="6">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="67" ht="20.05" customHeight="1">
-      <c r="A67" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B67" s="9">
-        <v>5.8</v>
-      </c>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" ht="20.05" customHeight="1">
-      <c r="A68" s="8">
+      <c r="A67" s="5">
         <v>2025</v>
       </c>
-      <c r="B68" s="9">
-        <v>5.8</v>
-      </c>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
+      <c r="B67" s="6">
+        <v>2.9</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>